<commit_message>
Vistas para roles y relleno de cargos vocal
</commit_message>
<xml_diff>
--- a/Rubrica Trabajo en grupo.xlsx
+++ b/Rubrica Trabajo en grupo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apere\Desktop\Programming\Oracle\ABD_Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1A6343-C891-4172-860F-033570D6C1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22602525-1412-40C3-96F5-D7579E749AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="87">
   <si>
     <t>Miscelanea</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t>Con los procedimientos RELLENA_EXAMEN, RELLENA_VIGILANCIA, RELLENAR_ASISTENCIA se itera por todos los alumnos, aulas, sedes y otros elementos de la base de datos, por lo que aseguramos que se cumplen las restricciones de integridad del modelo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                                                  </t>
   </si>
 </sst>
 </file>
@@ -919,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C334588-D4EB-43EC-8424-5ED08F8B2503}">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1777,7 +1780,7 @@
       <c r="D64" s="3"/>
       <c r="E64" s="23"/>
     </row>
-    <row r="65" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="C65" s="6" t="s">
         <v>1</v>
@@ -1793,7 +1796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="C66" s="6" t="s">
         <v>25</v>
@@ -1809,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6" t="s">
@@ -1826,12 +1829,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K68" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -1840,7 +1846,7 @@
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -1849,7 +1855,7 @@
         <v>1.2261904761904761</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Añadido manejo de expcepciones
</commit_message>
<xml_diff>
--- a/Rubrica Trabajo en grupo.xlsx
+++ b/Rubrica Trabajo en grupo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apere\Desktop\Programming\Oracle\ABD_Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22602525-1412-40C3-96F5-D7579E749AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07289741-113D-446D-9EBB-17F181048B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="94">
   <si>
     <t>Miscelanea</t>
   </si>
@@ -277,27 +277,6 @@
 FROM ESTUDIANTES_EXT;</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">insert into estudiante
-SELECT
- DNI, V_ESTUDIANTES.NOMBRE, APELLIDOS, TELEFONO, CORREO, CODIGO
-FROM V_ESTUDIANTES
-JOIN CENTRO ON V_ESTUDIANTES.CENTRO = CENTRO.NOMBRE;                      Se han insertado los datos de los estudiantes a partir de un join de la vista V_ESTUDIANTES y CENTRO, con esto conseguimos reunir la información pertinente para cada estudiante. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="4" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>FALTA TEMA VISTAS Y SEGURIDAD CON ROLES MARIO</t>
-    </r>
-  </si>
-  <si>
     <t>SEGURIDAD MARIO</t>
   </si>
   <si>
@@ -307,38 +286,69 @@
     <t>En el script de PEVAU está el procedimiento completo</t>
   </si>
   <si>
-    <t>Falta Gome por hacer</t>
-  </si>
-  <si>
     <t>En el script de PEVAU está el Trigger completo</t>
   </si>
   <si>
-    <t xml:space="preserve">Falta añadir COMMIT Y ROLLBACK EN EXCEPCIONES A TODOS LOS PROCEDIMIENTOS Y PAQUETES </t>
-  </si>
-  <si>
-    <t>Falta CONTROLAR EXCEPCIONES EN TODOS LOS PROCEDIMIENTOS (HACER ROLLBACK SI ALGO VA MAL QUIZAS)</t>
-  </si>
-  <si>
     <t>A porte de los datos proporcionados en el campus, se han creado los procedimientos RELLENA_EXAMEN, RELLENA_VIGILANCIA, RELLENAR_ASISTENCIA para popular de forma coherente las tablas sin datos de la base de datos. Se pueden encontrar en el .sql de la entrega.</t>
   </si>
   <si>
-    <t>Falta Chincoa por hacer</t>
-  </si>
-  <si>
-    <t>HAY QUE HACER ESTO AUN</t>
-  </si>
-  <si>
     <t>Con los procedimientos RELLENA_EXAMEN, RELLENA_VIGILANCIA, RELLENAR_ASISTENCIA se itera por todos los alumnos, aulas, sedes y otros elementos de la base de datos, por lo que aseguramos que se cumplen las restricciones de integridad del modelo.</t>
   </si>
   <si>
     <t xml:space="preserve">                                                                                                                                                                                  </t>
+  </si>
+  <si>
+    <t>CREATE TABLE estudiante (
+    dni           VARCHAR2(9) NOT NULL,
+    nombre        VARCHAR2(20) NOT NULL,
+    apellidos     VARCHAR2(25) NOT NULL,
+    telefono      VARCHAR2(15) NOT NULL ENCRYPT,
+    correo        VARCHAR2(50),
+    centro_codigo VARCHAR2(50) NOT NULL
+);  ATRIBUTO TELEFONO</t>
+  </si>
+  <si>
+    <t>Se consigue haciendo uso de las vistas: V_ESTUDIANTES y ASIGNACION_AULA_ESTUDIANTE</t>
+  </si>
+  <si>
+    <t>Se consigue con V_ASIGNACION_VIGILANTES y todas las que empiecen con V_RESPONSABLE_SEDE</t>
+  </si>
+  <si>
+    <t>Se consigue con V_ASIGNACION_VIGILANTES y V_CONTADOR_ESTUDIANTES_EXAMEN</t>
+  </si>
+  <si>
+    <t>Se consigue con V_ASIGNACION_VIGILANTES</t>
+  </si>
+  <si>
+    <t>Se consigue con V_VICERRECTORADO_ASIGNACION_R_SEDE y ASIGNACION_AULA_ESTUDIANTE y consultando sobre la tabla V_CONTADOR_ESTUDIANTES_EXAMEN</t>
+  </si>
+  <si>
+    <t>Paquete en la entrega de PEVAU.sql</t>
+  </si>
+  <si>
+    <t>REVISAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En fichero PEVAU.sql se puede ver </t>
+  </si>
+  <si>
+    <t>RELLENA_EXAMEN, RELLENAR_VIGILACIA, RELLENAR_ASISTENCIA, RELLENA_CARGOS_VOCAL</t>
+  </si>
+  <si>
+    <t>falta comprobar</t>
+  </si>
+  <si>
+    <t>ddl.sql</t>
+  </si>
+  <si>
+    <t>En Pevau.sql</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,36 +454,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="5" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -545,7 +528,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -605,13 +588,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -924,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C334588-D4EB-43EC-8424-5ED08F8B2503}">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,20 +1040,20 @@
       <c r="D10" s="6"/>
       <c r="E10" s="23"/>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="26" t="s">
-        <v>76</v>
+        <v>6</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1087,8 +1064,8 @@
       <c r="D12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="26" t="s">
-        <v>76</v>
+      <c r="E12" s="27" t="s">
+        <v>75</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
@@ -1139,20 +1116,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="21" t="s">
         <v>47</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="51.75" x14ac:dyDescent="0.25">
@@ -1161,14 +1138,14 @@
         <v>48</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>75</v>
+        <v>6</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>83</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="64.5" x14ac:dyDescent="0.25">
@@ -1177,14 +1154,14 @@
         <v>49</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>75</v>
+        <v>6</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>84</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
@@ -1193,14 +1170,14 @@
         <v>50</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>75</v>
+        <v>6</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1209,14 +1186,14 @@
         <v>51</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>75</v>
+        <v>6</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1238,7 +1215,9 @@
       <c r="D22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="23"/>
+      <c r="E22" s="23" t="s">
+        <v>87</v>
+      </c>
       <c r="F22">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1252,7 +1231,9 @@
       <c r="D23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="23"/>
+      <c r="E23" s="27" t="s">
+        <v>88</v>
+      </c>
       <c r="F23">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1285,7 +1266,7 @@
         <v>6</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F26">
         <f t="shared" ref="F26" si="1">IF(D26="SI",1,0)</f>
@@ -1301,7 +1282,7 @@
         <v>6</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F27">
         <f>IF(D27="SI",1,0)</f>
@@ -1317,7 +1298,7 @@
         <v>6</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F28">
         <f t="shared" ref="F28:F33" si="2">IF(D28="SI",1,0)</f>
@@ -1333,7 +1314,7 @@
         <v>6</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F29">
         <f t="shared" si="2"/>
@@ -1346,14 +1327,14 @@
         <v>58</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="27" t="s">
-        <v>78</v>
+        <v>6</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>76</v>
       </c>
       <c r="F30">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1362,14 +1343,14 @@
         <v>59</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="27" t="s">
-        <v>78</v>
+        <v>6</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>76</v>
       </c>
       <c r="F31">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1393,7 +1374,7 @@
         <v>6</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F33">
         <f t="shared" si="2"/>
@@ -1422,14 +1403,14 @@
         <v>33</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="28" t="s">
-        <v>80</v>
+        <v>6</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>93</v>
       </c>
       <c r="F36">
         <f t="shared" ref="F36" si="3">IF(D36="SI",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1444,19 +1425,19 @@
       <c r="D37" s="5"/>
       <c r="E37" s="23"/>
     </row>
-    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C38" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="28" t="s">
-        <v>81</v>
+        <v>6</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>93</v>
       </c>
       <c r="F38">
         <f t="shared" ref="F38" si="4">IF(D38="SI",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1477,7 +1458,7 @@
         <v>6</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F40">
         <f t="shared" ref="F40" si="5">IF(D40="SI",1,0)</f>
@@ -1507,7 +1488,7 @@
       <c r="E43" s="23"/>
       <c r="F43" s="25">
         <f>SUM(F6:F40)/24*2</f>
-        <v>1.0833333333333333</v>
+        <v>1.9166666666666667</v>
       </c>
       <c r="G43" t="s">
         <v>65</v>
@@ -1563,7 +1544,7 @@
         <v>7</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="F49">
         <f t="shared" ref="F49:F50" si="6">IF(D49="SI",1,0)</f>
@@ -1579,7 +1560,7 @@
         <v>7</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="F50">
         <f t="shared" si="6"/>
@@ -1610,12 +1591,14 @@
         <v>18</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E53" s="23"/>
+        <v>6</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>92</v>
+      </c>
       <c r="F53">
         <f t="shared" ref="F53:F54" si="7">IF(D53="SI",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1624,12 +1607,14 @@
         <v>19</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E54" s="23"/>
+        <v>6</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>92</v>
+      </c>
       <c r="F54">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1653,7 +1638,7 @@
         <v>7</v>
       </c>
       <c r="E56" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F56">
         <f t="shared" ref="F56:F63" si="8">IF(D56="SI",1,0)</f>
@@ -1669,7 +1654,7 @@
         <v>7</v>
       </c>
       <c r="E57" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F57">
         <f t="shared" si="8"/>
@@ -1685,7 +1670,7 @@
         <v>7</v>
       </c>
       <c r="E58" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F58">
         <f t="shared" si="8"/>
@@ -1701,7 +1686,7 @@
         <v>7</v>
       </c>
       <c r="E59" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F59">
         <f t="shared" si="8"/>
@@ -1717,7 +1702,7 @@
         <v>7</v>
       </c>
       <c r="E60" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F60">
         <f t="shared" si="8"/>
@@ -1733,7 +1718,7 @@
         <v>7</v>
       </c>
       <c r="E61" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F61">
         <f t="shared" si="8"/>
@@ -1758,14 +1743,14 @@
         <v>66</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E63" s="29" t="s">
-        <v>84</v>
+        <v>6</v>
+      </c>
+      <c r="E63" s="23" t="s">
+        <v>93</v>
       </c>
       <c r="F63">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1789,7 +1774,7 @@
         <v>6</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F65">
         <f t="shared" ref="F65:F67" si="9">IF(D65="SI",1,0)</f>
@@ -1802,14 +1787,14 @@
         <v>25</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E66" s="29" t="s">
-        <v>84</v>
+        <v>6</v>
+      </c>
+      <c r="E66" s="23" t="s">
+        <v>89</v>
       </c>
       <c r="F66">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1819,14 +1804,14 @@
         <v>35</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E67" s="29" t="s">
-        <v>84</v>
+        <v>6</v>
+      </c>
+      <c r="E67" s="23" t="s">
+        <v>90</v>
       </c>
       <c r="F67">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -1834,7 +1819,7 @@
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="K68" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -1843,7 +1828,7 @@
       <c r="C69" s="6"/>
       <c r="F69" s="25">
         <f>SUM(F49:F67)/14*2</f>
-        <v>0.14285714285714285</v>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -1852,7 +1837,7 @@
       <c r="C70" s="6"/>
       <c r="F70" s="25">
         <f>F69+F43</f>
-        <v>1.2261904761904761</v>
+        <v>2.7738095238095237</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TDE, encripción de nombre y apellidos de vocal
</commit_message>
<xml_diff>
--- a/Rubrica Trabajo en grupo.xlsx
+++ b/Rubrica Trabajo en grupo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apere\Desktop\Programming\Oracle\ABD_Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07289741-113D-446D-9EBB-17F181048B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64574D17-F586-4ADC-B6D5-7E2902273AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
@@ -348,7 +348,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,6 +461,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -528,7 +536,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -589,6 +597,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -901,7 +912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C334588-D4EB-43EC-8424-5ED08F8B2503}">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
@@ -1569,7 +1580,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
+      <c r="C51" s="28"/>
       <c r="D51" s="6"/>
       <c r="E51" s="23"/>
     </row>

</xml_diff>

<commit_message>
Entrega Final (parte obligatoria) falta trigger, vdp  y pk_ocupacion
</commit_message>
<xml_diff>
--- a/Rubrica Trabajo en grupo.xlsx
+++ b/Rubrica Trabajo en grupo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apere\Desktop\Programming\Oracle\ABD_Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64574D17-F586-4ADC-B6D5-7E2902273AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AFBF58-5F00-4947-A8BA-D5F38D9A03B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="95">
   <si>
     <t>Miscelanea</t>
   </si>
@@ -261,10 +261,6 @@
  centro, detalle
 FROM estudiantes_ext
  where dni is not null;</t>
-  </si>
-  <si>
-    <t>SELECT ui.index_name, ui.table_name, ui.tablespace_name
-FROM user_indexes ui;  Se han creado Índices de las claves primarias al generar el ddl  también; También se han generado índices a parte sobre la tabla estudiante, en los campos teléfono, centro_codigo y correo. Los indices nos permiten mejorar la velocidad de las consultas y para garantizar la unicidad. Nuestros indices son de tipo árbol  -B+ ya que practicamente en todos los campos donde nos interesa tener índices tenemos gran variabilidad de los datos.  Hay un índice de bitmap en el atributo centro_codigo de estudiante. Utilizamos este tipo de índice porque muchos estudiantes tienen asignado un mismo centro.</t>
   </si>
   <si>
     <t>CREATE MATERIALIZED VIEW VM_ESTUDIANTES
@@ -298,6 +294,45 @@
     <t xml:space="preserve">                                                                                                                                                                                  </t>
   </si>
   <si>
+    <t>Se consigue haciendo uso de las vistas: V_ESTUDIANTES y ASIGNACION_AULA_ESTUDIANTE</t>
+  </si>
+  <si>
+    <t>Se consigue con V_ASIGNACION_VIGILANTES y todas las que empiecen con V_RESPONSABLE_SEDE</t>
+  </si>
+  <si>
+    <t>Se consigue con V_ASIGNACION_VIGILANTES y V_CONTADOR_ESTUDIANTES_EXAMEN</t>
+  </si>
+  <si>
+    <t>Se consigue con V_ASIGNACION_VIGILANTES</t>
+  </si>
+  <si>
+    <t>Se consigue con V_VICERRECTORADO_ASIGNACION_R_SEDE y ASIGNACION_AULA_ESTUDIANTE y consultando sobre la tabla V_CONTADOR_ESTUDIANTES_EXAMEN</t>
+  </si>
+  <si>
+    <t>Paquete en la entrega de PEVAU.sql</t>
+  </si>
+  <si>
+    <t>REVISAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En fichero PEVAU.sql se puede ver </t>
+  </si>
+  <si>
+    <t>RELLENA_EXAMEN, RELLENAR_VIGILACIA, RELLENAR_ASISTENCIA, RELLENA_CARGOS_VOCAL</t>
+  </si>
+  <si>
+    <t>falta comprobar</t>
+  </si>
+  <si>
+    <t>ddl.sql</t>
+  </si>
+  <si>
+    <t>En Pevau.sql</t>
+  </si>
+  <si>
+    <t>En seguridad.sql viene el procedimiento para activarlo, y en el ddl se han encriptado las columnas.</t>
+  </si>
+  <si>
     <t>CREATE TABLE estudiante (
     dni           VARCHAR2(9) NOT NULL,
     nombre        VARCHAR2(20) NOT NULL,
@@ -305,43 +340,11 @@
     telefono      VARCHAR2(15) NOT NULL ENCRYPT,
     correo        VARCHAR2(50),
     centro_codigo VARCHAR2(50) NOT NULL
-);  ATRIBUTO TELEFONO</t>
-  </si>
-  <si>
-    <t>Se consigue haciendo uso de las vistas: V_ESTUDIANTES y ASIGNACION_AULA_ESTUDIANTE</t>
-  </si>
-  <si>
-    <t>Se consigue con V_ASIGNACION_VIGILANTES y todas las que empiecen con V_RESPONSABLE_SEDE</t>
-  </si>
-  <si>
-    <t>Se consigue con V_ASIGNACION_VIGILANTES y V_CONTADOR_ESTUDIANTES_EXAMEN</t>
-  </si>
-  <si>
-    <t>Se consigue con V_ASIGNACION_VIGILANTES</t>
-  </si>
-  <si>
-    <t>Se consigue con V_VICERRECTORADO_ASIGNACION_R_SEDE y ASIGNACION_AULA_ESTUDIANTE y consultando sobre la tabla V_CONTADOR_ESTUDIANTES_EXAMEN</t>
-  </si>
-  <si>
-    <t>Paquete en la entrega de PEVAU.sql</t>
-  </si>
-  <si>
-    <t>REVISAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En fichero PEVAU.sql se puede ver </t>
-  </si>
-  <si>
-    <t>RELLENA_EXAMEN, RELLENAR_VIGILACIA, RELLENAR_ASISTENCIA, RELLENA_CARGOS_VOCAL</t>
-  </si>
-  <si>
-    <t>falta comprobar</t>
-  </si>
-  <si>
-    <t>ddl.sql</t>
-  </si>
-  <si>
-    <t>En Pevau.sql</t>
+);  ATRIBUTO TELEFONO; también se ha cifrado el nombre y apellidos de los vocales</t>
+  </si>
+  <si>
+    <t>SELECT ui.index_name, ui.table_name, ui.tablespace_name
+FROM user_indexes ui;  Se han creado Índices de las claves primarias al generar el ddl  también; También se han generado índices a parte sobre la tabla estudiante, en los campos teléfono, y correo. Los indices nos permiten mejorar la velocidad de las consultas y para garantizar la unicidad. L a mayoría de nuestros indices son de tipo árbol  -B+ ya que practicamente en todos los campos donde nos interesa tener índices tenemos gran variabilidad de los datos.  Hay un índice de bitmap en el atributo centro_codigo de estudiante. Utilizamos este tipo de índice porque muchos estudiantes tienen asignado un mismo centro.</t>
   </si>
 </sst>
 </file>
@@ -536,7 +539,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -602,6 +605,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -912,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C334588-D4EB-43EC-8424-5ED08F8B2503}">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,9 +1020,9 @@
         <v>6</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8">
+        <v>94</v>
+      </c>
+      <c r="F8" s="29">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1051,7 +1055,7 @@
       <c r="D10" s="6"/>
       <c r="E10" s="23"/>
     </row>
-    <row r="11" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
         <v>43</v>
@@ -1060,7 +1064,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
@@ -1076,7 +1080,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
@@ -1120,7 +1124,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
@@ -1136,7 +1140,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
@@ -1152,7 +1156,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
@@ -1168,7 +1172,7 @@
         <v>6</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
@@ -1184,7 +1188,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
@@ -1200,7 +1204,7 @@
         <v>6</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
@@ -1227,7 +1231,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
@@ -1243,7 +1247,7 @@
         <v>6</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
@@ -1277,7 +1281,7 @@
         <v>6</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F26">
         <f t="shared" ref="F26" si="1">IF(D26="SI",1,0)</f>
@@ -1293,7 +1297,7 @@
         <v>6</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F27">
         <f>IF(D27="SI",1,0)</f>
@@ -1309,7 +1313,7 @@
         <v>6</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F28">
         <f t="shared" ref="F28:F33" si="2">IF(D28="SI",1,0)</f>
@@ -1325,7 +1329,7 @@
         <v>6</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F29">
         <f t="shared" si="2"/>
@@ -1341,7 +1345,7 @@
         <v>6</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F30">
         <f t="shared" si="2"/>
@@ -1357,7 +1361,7 @@
         <v>6</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F31">
         <f t="shared" si="2"/>
@@ -1385,7 +1389,7 @@
         <v>6</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F33">
         <f t="shared" si="2"/>
@@ -1417,7 +1421,7 @@
         <v>6</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F36">
         <f t="shared" ref="F36" si="3">IF(D36="SI",1,0)</f>
@@ -1444,7 +1448,7 @@
         <v>6</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F38">
         <f t="shared" ref="F38" si="4">IF(D38="SI",1,0)</f>
@@ -1469,7 +1473,7 @@
         <v>6</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F40">
         <f t="shared" ref="F40" si="5">IF(D40="SI",1,0)</f>
@@ -1555,7 +1559,7 @@
         <v>7</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F49">
         <f t="shared" ref="F49:F50" si="6">IF(D49="SI",1,0)</f>
@@ -1571,7 +1575,7 @@
         <v>7</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F50">
         <f t="shared" si="6"/>
@@ -1605,7 +1609,7 @@
         <v>6</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F53">
         <f t="shared" ref="F53:F54" si="7">IF(D53="SI",1,0)</f>
@@ -1621,7 +1625,7 @@
         <v>6</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F54">
         <f t="shared" si="7"/>
@@ -1649,7 +1653,7 @@
         <v>7</v>
       </c>
       <c r="E56" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F56">
         <f t="shared" ref="F56:F63" si="8">IF(D56="SI",1,0)</f>
@@ -1665,7 +1669,7 @@
         <v>7</v>
       </c>
       <c r="E57" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F57">
         <f t="shared" si="8"/>
@@ -1681,7 +1685,7 @@
         <v>7</v>
       </c>
       <c r="E58" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F58">
         <f t="shared" si="8"/>
@@ -1697,7 +1701,7 @@
         <v>7</v>
       </c>
       <c r="E59" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F59">
         <f t="shared" si="8"/>
@@ -1713,27 +1717,27 @@
         <v>7</v>
       </c>
       <c r="E60" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F60">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E61" s="26" t="s">
-        <v>74</v>
+        <v>6</v>
+      </c>
+      <c r="E61" s="23" t="s">
+        <v>92</v>
       </c>
       <c r="F61">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1757,7 +1761,7 @@
         <v>6</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F63">
         <f t="shared" si="8"/>
@@ -1785,7 +1789,7 @@
         <v>6</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F65">
         <f t="shared" ref="F65:F67" si="9">IF(D65="SI",1,0)</f>
@@ -1801,7 +1805,7 @@
         <v>6</v>
       </c>
       <c r="E66" s="23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F66">
         <f t="shared" si="9"/>
@@ -1818,7 +1822,7 @@
         <v>6</v>
       </c>
       <c r="E67" s="23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F67">
         <f t="shared" si="9"/>
@@ -1830,7 +1834,7 @@
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="K68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -1839,7 +1843,7 @@
       <c r="C69" s="6"/>
       <c r="F69" s="25">
         <f>SUM(F49:F67)/14*2</f>
-        <v>0.8571428571428571</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -1848,7 +1852,7 @@
       <c r="C70" s="6"/>
       <c r="F70" s="25">
         <f>F69+F43</f>
-        <v>2.7738095238095237</v>
+        <v>2.916666666666667</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mas notas para guion
</commit_message>
<xml_diff>
--- a/Rubrica Trabajo en grupo.xlsx
+++ b/Rubrica Trabajo en grupo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apere\Desktop\Programming\Oracle\ABD_Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AFBF58-5F00-4947-A8BA-D5F38D9A03B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA476EF9-CDDB-4E79-8194-85D07A3001AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -916,7 +916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C334588-D4EB-43EC-8424-5ED08F8B2503}">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
PK_OCUPACION intento de fix
</commit_message>
<xml_diff>
--- a/Rubrica Trabajo en grupo.xlsx
+++ b/Rubrica Trabajo en grupo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apere\Desktop\Programming\Oracle\ABD_Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA476EF9-CDDB-4E79-8194-85D07A3001AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0068DFC-3FE1-4CAF-89FB-E52C338F1578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="94">
   <si>
     <t>Miscelanea</t>
   </si>
@@ -310,9 +310,6 @@
   </si>
   <si>
     <t>Paquete en la entrega de PEVAU.sql</t>
-  </si>
-  <si>
-    <t>REVISAR</t>
   </si>
   <si>
     <t xml:space="preserve">En fichero PEVAU.sql se puede ver </t>
@@ -916,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C334588-D4EB-43EC-8424-5ED08F8B2503}">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,7 +1017,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F8" s="29">
         <f t="shared" si="0"/>
@@ -1064,7 +1061,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
@@ -1246,8 +1243,8 @@
       <c r="D23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="27" t="s">
-        <v>86</v>
+      <c r="E23" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
@@ -1421,7 +1418,7 @@
         <v>6</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F36">
         <f t="shared" ref="F36" si="3">IF(D36="SI",1,0)</f>
@@ -1448,7 +1445,7 @@
         <v>6</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F38">
         <f t="shared" ref="F38" si="4">IF(D38="SI",1,0)</f>
@@ -1559,7 +1556,7 @@
         <v>7</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F49">
         <f t="shared" ref="F49:F50" si="6">IF(D49="SI",1,0)</f>
@@ -1575,7 +1572,7 @@
         <v>7</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F50">
         <f t="shared" si="6"/>
@@ -1609,7 +1606,7 @@
         <v>6</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F53">
         <f t="shared" ref="F53:F54" si="7">IF(D53="SI",1,0)</f>
@@ -1625,7 +1622,7 @@
         <v>6</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F54">
         <f t="shared" si="7"/>
@@ -1733,7 +1730,7 @@
         <v>6</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F61">
         <f t="shared" si="8"/>
@@ -1761,7 +1758,7 @@
         <v>6</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F63">
         <f t="shared" si="8"/>
@@ -1805,7 +1802,7 @@
         <v>6</v>
       </c>
       <c r="E66" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F66">
         <f t="shared" si="9"/>
@@ -1822,7 +1819,7 @@
         <v>6</v>
       </c>
       <c r="E67" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F67">
         <f t="shared" si="9"/>

</xml_diff>

<commit_message>
Añadidos roles y privilegios en system.sql
</commit_message>
<xml_diff>
--- a/Rubrica Trabajo en grupo.xlsx
+++ b/Rubrica Trabajo en grupo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apere\Desktop\Programming\Oracle\ABD_Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0068DFC-3FE1-4CAF-89FB-E52C338F1578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2417B235-3B09-40EF-A57B-C116F461A013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
@@ -306,9 +306,6 @@
     <t>Se consigue con V_ASIGNACION_VIGILANTES</t>
   </si>
   <si>
-    <t>Se consigue con V_VICERRECTORADO_ASIGNACION_R_SEDE y ASIGNACION_AULA_ESTUDIANTE y consultando sobre la tabla V_CONTADOR_ESTUDIANTES_EXAMEN</t>
-  </si>
-  <si>
     <t>Paquete en la entrega de PEVAU.sql</t>
   </si>
   <si>
@@ -342,6 +339,9 @@
   <si>
     <t>SELECT ui.index_name, ui.table_name, ui.tablespace_name
 FROM user_indexes ui;  Se han creado Índices de las claves primarias al generar el ddl  también; También se han generado índices a parte sobre la tabla estudiante, en los campos teléfono, y correo. Los indices nos permiten mejorar la velocidad de las consultas y para garantizar la unicidad. L a mayoría de nuestros indices son de tipo árbol  -B+ ya que practicamente en todos los campos donde nos interesa tener índices tenemos gran variabilidad de los datos.  Hay un índice de bitmap en el atributo centro_codigo de estudiante. Utilizamos este tipo de índice porque muchos estudiantes tienen asignado un mismo centro.</t>
+  </si>
+  <si>
+    <t>Se consigue con V_RESPONSABLE_SEDE_ASIGNACION_EXAMENES, V_RESPONSABLE_SEDE_ASISTENCIA, V_RESPONSABLE_SEDE_AULAS,  V_RESPONSABLE_SEDE_SEDES,  ASIGNACION_AULA_ESTUDIANTE y consultando sobre la vista V_CONTADOR_ESTUDIANTES_EXAMEN</t>
   </si>
 </sst>
 </file>
@@ -914,7 +914,7 @@
   <dimension ref="A1:K71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,7 +1017,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F8" s="29">
         <f t="shared" si="0"/>
@@ -1061,7 +1061,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
@@ -1192,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="21" t="s">
         <v>51</v>
@@ -1201,7 +1201,7 @@
         <v>6</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
@@ -1228,7 +1228,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
@@ -1244,7 +1244,7 @@
         <v>6</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
@@ -1418,7 +1418,7 @@
         <v>6</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F36">
         <f t="shared" ref="F36" si="3">IF(D36="SI",1,0)</f>
@@ -1445,7 +1445,7 @@
         <v>6</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F38">
         <f t="shared" ref="F38" si="4">IF(D38="SI",1,0)</f>
@@ -1556,7 +1556,7 @@
         <v>7</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F49">
         <f t="shared" ref="F49:F50" si="6">IF(D49="SI",1,0)</f>
@@ -1572,7 +1572,7 @@
         <v>7</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F50">
         <f t="shared" si="6"/>
@@ -1606,7 +1606,7 @@
         <v>6</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F53">
         <f t="shared" ref="F53:F54" si="7">IF(D53="SI",1,0)</f>
@@ -1622,7 +1622,7 @@
         <v>6</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F54">
         <f t="shared" si="7"/>
@@ -1730,7 +1730,7 @@
         <v>6</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F61">
         <f t="shared" si="8"/>
@@ -1758,7 +1758,7 @@
         <v>6</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F63">
         <f t="shared" si="8"/>
@@ -1802,7 +1802,7 @@
         <v>6</v>
       </c>
       <c r="E66" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F66">
         <f t="shared" si="9"/>
@@ -1819,7 +1819,7 @@
         <v>6</v>
       </c>
       <c r="E67" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F67">
         <f t="shared" si="9"/>

</xml_diff>

<commit_message>
VPD Y CREACION DE USUARIOS CON ROLES FUNCIONANDO
</commit_message>
<xml_diff>
--- a/Rubrica Trabajo en grupo.xlsx
+++ b/Rubrica Trabajo en grupo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apere\Desktop\Programming\Oracle\ABD_Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2417B235-3B09-40EF-A57B-C116F461A013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C5D314-AA34-4FAE-86D6-6A6A2070AE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="95">
   <si>
     <t>Miscelanea</t>
   </si>
@@ -276,9 +276,6 @@
     <t>SEGURIDAD MARIO</t>
   </si>
   <si>
-    <t>SEGURIDAD CIFRADO</t>
-  </si>
-  <si>
     <t>En el script de PEVAU está el procedimiento completo</t>
   </si>
   <si>
@@ -286,9 +283,6 @@
   </si>
   <si>
     <t>A porte de los datos proporcionados en el campus, se han creado los procedimientos RELLENA_EXAMEN, RELLENA_VIGILANCIA, RELLENAR_ASISTENCIA para popular de forma coherente las tablas sin datos de la base de datos. Se pueden encontrar en el .sql de la entrega.</t>
-  </si>
-  <si>
-    <t>Con los procedimientos RELLENA_EXAMEN, RELLENA_VIGILANCIA, RELLENAR_ASISTENCIA se itera por todos los alumnos, aulas, sedes y otros elementos de la base de datos, por lo que aseguramos que se cumplen las restricciones de integridad del modelo.</t>
   </si>
   <si>
     <t xml:space="preserve">                                                                                                                                                                                  </t>
@@ -342,6 +336,15 @@
   </si>
   <si>
     <t>Se consigue con V_RESPONSABLE_SEDE_ASIGNACION_EXAMENES, V_RESPONSABLE_SEDE_ASISTENCIA, V_RESPONSABLE_SEDE_AULAS,  V_RESPONSABLE_SEDE_SEDES,  ASIGNACION_AULA_ESTUDIANTE y consultando sobre la vista V_CONTADOR_ESTUDIANTES_EXAMEN</t>
+  </si>
+  <si>
+    <t>Con los procedimientos RELLENA_EXAMEN, RELLENA_VIGILANCIA, RELLENAR_ASISTENCIA,RELLENA CARGOS VOCAL, se itera por todos los alumnos, aulas, sedes y otros elementos de la base de datos, por lo que aseguramos que se cumplen las restricciones de integridad del modelo.</t>
+  </si>
+  <si>
+    <t>En system.sql</t>
+  </si>
+  <si>
+    <t>En system.sql y seguridad.sql</t>
   </si>
 </sst>
 </file>
@@ -913,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C334588-D4EB-43EC-8424-5ED08F8B2503}">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,7 +1020,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F8" s="29">
         <f t="shared" si="0"/>
@@ -1061,7 +1064,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
@@ -1074,14 +1077,14 @@
         <v>44</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>74</v>
+        <v>6</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>94</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1137,7 +1140,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
@@ -1153,7 +1156,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
@@ -1169,7 +1172,7 @@
         <v>6</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
@@ -1185,7 +1188,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
@@ -1201,7 +1204,7 @@
         <v>6</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
@@ -1228,7 +1231,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
@@ -1244,7 +1247,7 @@
         <v>6</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
@@ -1278,7 +1281,7 @@
         <v>6</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F26">
         <f t="shared" ref="F26" si="1">IF(D26="SI",1,0)</f>
@@ -1294,7 +1297,7 @@
         <v>6</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F27">
         <f>IF(D27="SI",1,0)</f>
@@ -1310,7 +1313,7 @@
         <v>6</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F28">
         <f t="shared" ref="F28:F33" si="2">IF(D28="SI",1,0)</f>
@@ -1326,7 +1329,7 @@
         <v>6</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F29">
         <f t="shared" si="2"/>
@@ -1342,7 +1345,7 @@
         <v>6</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F30">
         <f t="shared" si="2"/>
@@ -1358,7 +1361,7 @@
         <v>6</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F31">
         <f t="shared" si="2"/>
@@ -1386,7 +1389,7 @@
         <v>6</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F33">
         <f t="shared" si="2"/>
@@ -1418,7 +1421,7 @@
         <v>6</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F36">
         <f t="shared" ref="F36" si="3">IF(D36="SI",1,0)</f>
@@ -1445,7 +1448,7 @@
         <v>6</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F38">
         <f t="shared" ref="F38" si="4">IF(D38="SI",1,0)</f>
@@ -1470,7 +1473,7 @@
         <v>6</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F40">
         <f t="shared" ref="F40" si="5">IF(D40="SI",1,0)</f>
@@ -1500,7 +1503,7 @@
       <c r="E43" s="23"/>
       <c r="F43" s="25">
         <f>SUM(F6:F40)/24*2</f>
-        <v>1.9166666666666667</v>
+        <v>2</v>
       </c>
       <c r="G43" t="s">
         <v>65</v>
@@ -1556,7 +1559,7 @@
         <v>7</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F49">
         <f t="shared" ref="F49:F50" si="6">IF(D49="SI",1,0)</f>
@@ -1572,7 +1575,7 @@
         <v>7</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F50">
         <f t="shared" si="6"/>
@@ -1606,7 +1609,7 @@
         <v>6</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F53">
         <f t="shared" ref="F53:F54" si="7">IF(D53="SI",1,0)</f>
@@ -1622,7 +1625,7 @@
         <v>6</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F54">
         <f t="shared" si="7"/>
@@ -1647,14 +1650,14 @@
         <v>21</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E56" s="26" t="s">
-        <v>73</v>
+        <v>6</v>
+      </c>
+      <c r="E56" s="23" t="s">
+        <v>93</v>
       </c>
       <c r="F56">
         <f t="shared" ref="F56:F63" si="8">IF(D56="SI",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1730,7 +1733,7 @@
         <v>6</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F61">
         <f t="shared" si="8"/>
@@ -1758,7 +1761,7 @@
         <v>6</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F63">
         <f t="shared" si="8"/>
@@ -1777,7 +1780,7 @@
       <c r="D64" s="3"/>
       <c r="E64" s="23"/>
     </row>
-    <row r="65" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="C65" s="6" t="s">
         <v>1</v>
@@ -1786,7 +1789,7 @@
         <v>6</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="F65">
         <f t="shared" ref="F65:F67" si="9">IF(D65="SI",1,0)</f>
@@ -1802,7 +1805,7 @@
         <v>6</v>
       </c>
       <c r="E66" s="23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F66">
         <f t="shared" si="9"/>
@@ -1819,7 +1822,7 @@
         <v>6</v>
       </c>
       <c r="E67" s="23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F67">
         <f t="shared" si="9"/>
@@ -1831,7 +1834,7 @@
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="K68" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -1840,7 +1843,7 @@
       <c r="C69" s="6"/>
       <c r="F69" s="25">
         <f>SUM(F49:F67)/14*2</f>
-        <v>1</v>
+        <v>1.1428571428571428</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -1849,7 +1852,7 @@
       <c r="C70" s="6"/>
       <c r="F70" s="25">
         <f>F69+F43</f>
-        <v>2.916666666666667</v>
+        <v>3.1428571428571428</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Solucionado aleatoriedad de asistencia
</commit_message>
<xml_diff>
--- a/Rubrica Trabajo en grupo.xlsx
+++ b/Rubrica Trabajo en grupo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apere\Desktop\Programming\Oracle\ABD_Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C5D314-AA34-4FAE-86D6-6A6A2070AE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE7E296-ACD2-4EAC-8E4F-1702E1D75769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="97">
   <si>
     <t>Miscelanea</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>En system.sql y seguridad.sql</t>
+  </si>
+  <si>
+    <t>En system.sql y paquete de creación de usuarios</t>
+  </si>
+  <si>
+    <t>En paquete de creación de usuarios</t>
   </si>
 </sst>
 </file>
@@ -916,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C334588-D4EB-43EC-8424-5ED08F8B2503}">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,14 +1672,14 @@
         <v>22</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E57" s="26" t="s">
-        <v>73</v>
+        <v>6</v>
+      </c>
+      <c r="E57" s="23" t="s">
+        <v>96</v>
       </c>
       <c r="F57">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1682,14 +1688,14 @@
         <v>23</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" s="26" t="s">
-        <v>73</v>
+        <v>6</v>
+      </c>
+      <c r="E58" s="23" t="s">
+        <v>95</v>
       </c>
       <c r="F58">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1843,7 +1849,7 @@
       <c r="C69" s="6"/>
       <c r="F69" s="25">
         <f>SUM(F49:F67)/14*2</f>
-        <v>1.1428571428571428</v>
+        <v>1.4285714285714286</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -1852,7 +1858,7 @@
       <c r="C70" s="6"/>
       <c r="F70" s="25">
         <f>F69+F43</f>
-        <v>3.1428571428571428</v>
+        <v>3.4285714285714288</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cambio de fechas, añadidos elementos a entrega de seguridad, creacion de ussuario para vicerrectorado
</commit_message>
<xml_diff>
--- a/Rubrica Trabajo en grupo.xlsx
+++ b/Rubrica Trabajo en grupo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apere\Desktop\Programming\Oracle\ABD_Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE7E296-ACD2-4EAC-8E4F-1702E1D75769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB71C709-DC38-4319-A8C8-8CB1D8CACCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -282,9 +282,6 @@
     <t>En el script de PEVAU está el Trigger completo</t>
   </si>
   <si>
-    <t>A porte de los datos proporcionados en el campus, se han creado los procedimientos RELLENA_EXAMEN, RELLENA_VIGILANCIA, RELLENAR_ASISTENCIA para popular de forma coherente las tablas sin datos de la base de datos. Se pueden encontrar en el .sql de la entrega.</t>
-  </si>
-  <si>
     <t xml:space="preserve">                                                                                                                                                                                  </t>
   </si>
   <si>
@@ -351,6 +348,9 @@
   </si>
   <si>
     <t>En paquete de creación de usuarios</t>
+  </si>
+  <si>
+    <t>A parte de los datos proporcionados en el campus, se han creado los procedimientos RELLENA_EXAMEN, RELLENA_VIGILANCIA, RELLENAR_ASISTENCIA para popular de forma coherente las tablas sin datos de la base de datos. Se pueden encontrar en el .sql de la entrega.</t>
   </si>
 </sst>
 </file>
@@ -922,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C334588-D4EB-43EC-8424-5ED08F8B2503}">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1026,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F8" s="29">
         <f t="shared" si="0"/>
@@ -1070,7 +1070,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
@@ -1086,7 +1086,7 @@
         <v>6</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
@@ -1146,7 +1146,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
@@ -1162,7 +1162,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
@@ -1178,7 +1178,7 @@
         <v>6</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
@@ -1194,7 +1194,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
@@ -1210,7 +1210,7 @@
         <v>6</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
@@ -1237,7 +1237,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
@@ -1253,7 +1253,7 @@
         <v>6</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
@@ -1427,7 +1427,7 @@
         <v>6</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F36">
         <f t="shared" ref="F36" si="3">IF(D36="SI",1,0)</f>
@@ -1454,7 +1454,7 @@
         <v>6</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F38">
         <f t="shared" ref="F38" si="4">IF(D38="SI",1,0)</f>
@@ -1479,7 +1479,7 @@
         <v>6</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="F40">
         <f t="shared" ref="F40" si="5">IF(D40="SI",1,0)</f>
@@ -1565,7 +1565,7 @@
         <v>7</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F49">
         <f t="shared" ref="F49:F50" si="6">IF(D49="SI",1,0)</f>
@@ -1581,7 +1581,7 @@
         <v>7</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F50">
         <f t="shared" si="6"/>
@@ -1615,7 +1615,7 @@
         <v>6</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F53">
         <f t="shared" ref="F53:F54" si="7">IF(D53="SI",1,0)</f>
@@ -1631,7 +1631,7 @@
         <v>6</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F54">
         <f t="shared" si="7"/>
@@ -1659,7 +1659,7 @@
         <v>6</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F56">
         <f t="shared" ref="F56:F63" si="8">IF(D56="SI",1,0)</f>
@@ -1675,7 +1675,7 @@
         <v>6</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F57">
         <f t="shared" si="8"/>
@@ -1691,7 +1691,7 @@
         <v>6</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F58">
         <f t="shared" si="8"/>
@@ -1739,7 +1739,7 @@
         <v>6</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F61">
         <f t="shared" si="8"/>
@@ -1767,7 +1767,7 @@
         <v>6</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F63">
         <f t="shared" si="8"/>
@@ -1795,7 +1795,7 @@
         <v>6</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F65">
         <f t="shared" ref="F65:F67" si="9">IF(D65="SI",1,0)</f>
@@ -1811,7 +1811,7 @@
         <v>6</v>
       </c>
       <c r="E66" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F66">
         <f t="shared" si="9"/>
@@ -1828,7 +1828,7 @@
         <v>6</v>
       </c>
       <c r="E67" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F67">
         <f t="shared" si="9"/>
@@ -1840,7 +1840,7 @@
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="K68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cambios para entrega final
</commit_message>
<xml_diff>
--- a/Rubrica Trabajo en grupo.xlsx
+++ b/Rubrica Trabajo en grupo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apere\Desktop\Programming\Oracle\ABD_Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18A2D4F-0F88-4689-816D-1051C18219F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AD11B8-8D4E-4C37-A77A-467CBC933662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
@@ -925,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C334588-D4EB-43EC-8424-5ED08F8B2503}">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1881,7 +1881,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{092406BF-548E-4837-A087-DD29E26D8086}">
           <x14:formula1>
             <xm:f>Hoja2!$A$2:$A$3</xm:f>

</xml_diff>